<commit_message>
resave on the first list
</commit_message>
<xml_diff>
--- a/ТМОГИ.2016.осень.xlsx
+++ b/ТМОГИ.2016.осень.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1620" windowWidth="12504" windowHeight="7920" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="1620" windowWidth="12510" windowHeight="7920"/>
   </bookViews>
   <sheets>
     <sheet name="Сводная таблица" sheetId="1" r:id="rId1"/>
@@ -1804,39 +1804,39 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:II135"/>
   <sheetViews>
-    <sheetView topLeftCell="A65" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:II4"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="BI9" sqref="BI9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.4" zeroHeight="1"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15" zeroHeight="1"/>
   <cols>
-    <col min="1" max="1" width="4.33203125" customWidth="1"/>
-    <col min="2" max="2" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="3.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.6640625" customWidth="1"/>
-    <col min="5" max="5" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.44140625" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="5.88671875" style="35" customWidth="1"/>
-    <col min="8" max="8" width="5.6640625" style="35" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="4.88671875" style="35" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="5.44140625" style="35" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="4.33203125" style="35" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="4.88671875" hidden="1" customWidth="1"/>
-    <col min="13" max="14" width="4.5546875" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="4.28515625" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="3.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.42578125" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="5.85546875" style="35" customWidth="1"/>
+    <col min="8" max="8" width="5.7109375" style="35" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="4.85546875" style="35" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="5.42578125" style="35" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="4.28515625" style="35" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="4.85546875" hidden="1" customWidth="1"/>
+    <col min="13" max="14" width="4.5703125" hidden="1" customWidth="1"/>
     <col min="15" max="15" width="5" hidden="1" customWidth="1"/>
-    <col min="16" max="16" width="5.109375" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="5.140625" hidden="1" customWidth="1"/>
     <col min="17" max="17" width="5" hidden="1" customWidth="1"/>
-    <col min="18" max="18" width="4.5546875" hidden="1" customWidth="1"/>
+    <col min="18" max="18" width="4.5703125" hidden="1" customWidth="1"/>
     <col min="19" max="19" width="5" hidden="1" customWidth="1"/>
-    <col min="20" max="20" width="4.5546875" hidden="1" customWidth="1"/>
-    <col min="21" max="22" width="3.33203125" hidden="1" customWidth="1"/>
-    <col min="23" max="24" width="3.33203125" customWidth="1"/>
+    <col min="20" max="20" width="4.5703125" hidden="1" customWidth="1"/>
+    <col min="21" max="22" width="3.28515625" hidden="1" customWidth="1"/>
+    <col min="23" max="24" width="3.28515625" customWidth="1"/>
     <col min="25" max="25" width="4" customWidth="1"/>
-    <col min="26" max="26" width="4.109375" bestFit="1" customWidth="1"/>
-    <col min="27" max="32" width="3.33203125" customWidth="1"/>
-    <col min="33" max="58" width="3.33203125" hidden="1" customWidth="1"/>
-    <col min="59" max="59" width="4.33203125" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="27" max="32" width="3.28515625" customWidth="1"/>
+    <col min="33" max="58" width="3.28515625" hidden="1" customWidth="1"/>
+    <col min="59" max="59" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="5.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:243" ht="20.100000000000001" customHeight="1">
@@ -2086,7 +2086,7 @@
       <c r="IH1" s="145"/>
       <c r="II1" s="145"/>
     </row>
-    <row r="2" spans="1:243" ht="15" thickBot="1">
+    <row r="2" spans="1:243" ht="15.75" thickBot="1">
       <c r="B2" s="106">
         <f>DATE(2016,9,1)</f>
         <v>42614</v>
@@ -2337,7 +2337,7 @@
       <c r="BG3" s="3"/>
       <c r="BH3" s="3"/>
     </row>
-    <row r="4" spans="1:243" ht="43.2">
+    <row r="4" spans="1:243" ht="45">
       <c r="A4" s="147"/>
       <c r="B4" s="142"/>
       <c r="C4" s="144"/>
@@ -6459,7 +6459,7 @@
         <v>4.4403330249768729</v>
       </c>
     </row>
-    <row r="46" spans="1:60" ht="15" thickBot="1">
+    <row r="46" spans="1:60" ht="15.75" thickBot="1">
       <c r="A46" s="24">
         <v>42</v>
       </c>
@@ -6765,7 +6765,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:60" ht="15" thickBot="1">
+    <row r="50" spans="1:60" ht="15.75" thickBot="1">
       <c r="G50"/>
       <c r="H50"/>
       <c r="I50"/>
@@ -6961,7 +6961,7 @@
       <c r="BG51" s="24"/>
       <c r="BH51" s="24"/>
     </row>
-    <row r="52" spans="1:60" ht="43.2">
+    <row r="52" spans="1:60" ht="45">
       <c r="A52" s="148"/>
       <c r="B52" s="142"/>
       <c r="C52" s="144"/>
@@ -13117,7 +13117,7 @@
       <c r="BG128" s="41"/>
       <c r="BH128" s="11"/>
     </row>
-    <row r="129" spans="1:60" ht="15" hidden="1" thickBot="1">
+    <row r="129" spans="1:60" ht="15.75" hidden="1" thickBot="1">
       <c r="A129" s="18"/>
       <c r="B129" s="16"/>
       <c r="C129" s="109"/>
@@ -13248,11 +13248,6 @@
     <sortCondition descending="1" ref="BH53:BH94"/>
   </sortState>
   <mergeCells count="17">
-    <mergeCell ref="N3:U3"/>
-    <mergeCell ref="G51:M51"/>
-    <mergeCell ref="N51:U51"/>
-    <mergeCell ref="B51:B52"/>
-    <mergeCell ref="C51:C52"/>
     <mergeCell ref="A1:II1"/>
     <mergeCell ref="F3:F4"/>
     <mergeCell ref="A3:A4"/>
@@ -13265,6 +13260,11 @@
     <mergeCell ref="E51:E52"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="G3:M3"/>
+    <mergeCell ref="N3:U3"/>
+    <mergeCell ref="G51:M51"/>
+    <mergeCell ref="N51:U51"/>
+    <mergeCell ref="B51:B52"/>
+    <mergeCell ref="C51:C52"/>
   </mergeCells>
   <pageMargins left="0.19685039370078999" right="0.19" top="0.31496062992126" bottom="0.74803149606299002" header="0.31496062992126" footer="0.31496062992126"/>
   <pageSetup paperSize="9" scale="90" orientation="landscape" r:id="rId1"/>
@@ -13279,19 +13279,19 @@
       <selection activeCell="M31" sqref="M31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="3.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="21.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="3.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:255" ht="20.100000000000001" customHeight="1">
@@ -13553,7 +13553,7 @@
       <c r="IT1" s="145"/>
       <c r="IU1" s="145"/>
     </row>
-    <row r="2" spans="1:255" ht="15" thickBot="1">
+    <row r="2" spans="1:255" ht="15.75" thickBot="1">
       <c r="A2" s="153" t="str">
         <f>'Сводная таблица'!D2</f>
         <v>Группы 114 05 115 - 114 05 215</v>
@@ -13610,7 +13610,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:255" ht="15" thickBot="1">
+    <row r="4" spans="1:255" ht="15.75" thickBot="1">
       <c r="A4" s="155"/>
       <c r="B4" s="157"/>
       <c r="C4" s="159"/>
@@ -15386,7 +15386,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:11" s="77" customFormat="1" ht="15" thickBot="1">
+    <row r="46" spans="1:11" s="77" customFormat="1" ht="15.75" thickBot="1">
       <c r="A46" s="79">
         <f>'Сводная таблица'!A46:A47</f>
         <v>42</v>
@@ -15511,13 +15511,13 @@
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="31.33203125" style="102" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.6640625" style="4" customWidth="1"/>
-    <col min="3" max="27" width="9.109375" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="9.109375" style="63"/>
+    <col min="1" max="1" width="31.28515625" style="102" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" style="4" customWidth="1"/>
+    <col min="3" max="27" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="9.140625" style="63"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:256" ht="20.100000000000001" customHeight="1">
@@ -42670,19 +42670,19 @@
       <selection activeCell="V23" sqref="V23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="3.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="21.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="3.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:255" ht="20.100000000000001" customHeight="1">
@@ -42944,7 +42944,7 @@
       <c r="IT1" s="145"/>
       <c r="IU1" s="145"/>
     </row>
-    <row r="2" spans="1:255" ht="15" thickBot="1">
+    <row r="2" spans="1:255" ht="15.75" thickBot="1">
       <c r="A2" s="153" t="str">
         <f>'Сводная таблица'!D2</f>
         <v>Группы 114 05 115 - 114 05 215</v>
@@ -43001,7 +43001,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:255" ht="15" thickBot="1">
+    <row r="4" spans="1:255" ht="15.75" thickBot="1">
       <c r="A4" s="155"/>
       <c r="B4" s="157"/>
       <c r="C4" s="159"/>
@@ -44756,7 +44756,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:11" s="77" customFormat="1" ht="15" thickBot="1">
+    <row r="46" spans="1:11" s="77" customFormat="1" ht="15.75" thickBot="1">
       <c r="A46" s="79">
         <f>'Сводная таблица'!A46:A47</f>
         <v>42</v>
@@ -44877,23 +44877,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:IU52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N18" sqref="N18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="3.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="21.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="3.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:255" ht="20.100000000000001" customHeight="1">
@@ -45155,7 +45155,7 @@
       <c r="IT1" s="145"/>
       <c r="IU1" s="145"/>
     </row>
-    <row r="2" spans="1:255" ht="15" thickBot="1">
+    <row r="2" spans="1:255" ht="15.75" thickBot="1">
       <c r="A2" s="153" t="str">
         <f>'Сводная таблица'!D2</f>
         <v>Группы 114 05 115 - 114 05 215</v>
@@ -45212,7 +45212,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:255" ht="15" thickBot="1">
+    <row r="4" spans="1:255" ht="15.75" thickBot="1">
       <c r="A4" s="155"/>
       <c r="B4" s="157"/>
       <c r="C4" s="159"/>
@@ -46988,7 +46988,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:11" s="77" customFormat="1" ht="15" thickBot="1">
+    <row r="46" spans="1:11" s="77" customFormat="1" ht="15.75" thickBot="1">
       <c r="A46" s="79">
         <f>'Сводная таблица'!A46:A47</f>
         <v>42</v>
@@ -47113,12 +47113,12 @@
       <selection activeCell="K5" sqref="K5:K46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:256" ht="20.100000000000001" customHeight="1">
@@ -47381,7 +47381,7 @@
       <c r="IU1" s="145"/>
       <c r="IV1" s="145"/>
     </row>
-    <row r="2" spans="1:256" ht="15" thickBot="1">
+    <row r="2" spans="1:256" ht="15.75" thickBot="1">
       <c r="A2" s="153" t="str">
         <f>'Сводная таблица'!D2</f>
         <v>Группы 114 05 115 - 114 05 215</v>
@@ -47438,7 +47438,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:256" ht="15" thickBot="1">
+    <row r="4" spans="1:256" ht="15.75" thickBot="1">
       <c r="A4" s="155"/>
       <c r="B4" s="157"/>
       <c r="C4" s="159"/>
@@ -49214,7 +49214,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:11" s="77" customFormat="1" ht="15" thickBot="1">
+    <row r="46" spans="1:11" s="77" customFormat="1" ht="15.75" thickBot="1">
       <c r="A46" s="79">
         <f>'Сводная таблица'!A46:A47</f>
         <v>42</v>
@@ -49285,12 +49285,12 @@
       <selection activeCell="K5" sqref="K5:K46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:256" ht="20.100000000000001" customHeight="1">
@@ -49553,7 +49553,7 @@
       <c r="IU1" s="145"/>
       <c r="IV1" s="145"/>
     </row>
-    <row r="2" spans="1:256" ht="15" thickBot="1">
+    <row r="2" spans="1:256" ht="15.75" thickBot="1">
       <c r="A2" s="153" t="str">
         <f>'Сводная таблица'!D2</f>
         <v>Группы 114 05 115 - 114 05 215</v>
@@ -49610,7 +49610,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:256" ht="15" thickBot="1">
+    <row r="4" spans="1:256" ht="15.75" thickBot="1">
       <c r="A4" s="155"/>
       <c r="B4" s="157"/>
       <c r="C4" s="159"/>
@@ -51386,7 +51386,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:11" s="77" customFormat="1" ht="15" thickBot="1">
+    <row r="46" spans="1:11" s="77" customFormat="1" ht="15.75" thickBot="1">
       <c r="A46" s="79">
         <f>'Сводная таблица'!A46:A47</f>
         <v>42</v>
@@ -51457,12 +51457,12 @@
       <selection activeCell="K5" sqref="K5:K46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:256" ht="20.100000000000001" customHeight="1">
@@ -51725,7 +51725,7 @@
       <c r="IU1" s="145"/>
       <c r="IV1" s="145"/>
     </row>
-    <row r="2" spans="1:256" ht="15" thickBot="1">
+    <row r="2" spans="1:256" ht="15.75" thickBot="1">
       <c r="A2" s="153" t="str">
         <f>'Сводная таблица'!D2</f>
         <v>Группы 114 05 115 - 114 05 215</v>
@@ -51782,7 +51782,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:256" ht="15" thickBot="1">
+    <row r="4" spans="1:256" ht="15.75" thickBot="1">
       <c r="A4" s="155"/>
       <c r="B4" s="157"/>
       <c r="C4" s="159"/>
@@ -53558,7 +53558,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:11" s="77" customFormat="1" ht="15" thickBot="1">
+    <row r="46" spans="1:11" s="77" customFormat="1" ht="15.75" thickBot="1">
       <c r="A46" s="79">
         <f>'Сводная таблица'!A46:A47</f>
         <v>42</v>
@@ -53629,12 +53629,12 @@
       <selection activeCell="I50" sqref="I50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:256" ht="20.100000000000001" customHeight="1">
@@ -53897,7 +53897,7 @@
       <c r="IU1" s="145"/>
       <c r="IV1" s="145"/>
     </row>
-    <row r="2" spans="1:256" ht="15" thickBot="1">
+    <row r="2" spans="1:256" ht="15.75" thickBot="1">
       <c r="A2" s="153" t="str">
         <f>'Сводная таблица'!D2</f>
         <v>Группы 114 05 115 - 114 05 215</v>
@@ -53954,7 +53954,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:256" ht="15" thickBot="1">
+    <row r="4" spans="1:256" ht="15.75" thickBot="1">
       <c r="A4" s="155"/>
       <c r="B4" s="157"/>
       <c r="C4" s="159"/>
@@ -55730,7 +55730,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:11" s="77" customFormat="1" ht="15" thickBot="1">
+    <row r="46" spans="1:11" s="77" customFormat="1" ht="15.75" thickBot="1">
       <c r="A46" s="79">
         <f>'Сводная таблица'!A46:A47</f>
         <v>42</v>
@@ -55801,12 +55801,12 @@
       <selection activeCell="K5" sqref="K5:K46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:256" ht="20.100000000000001" customHeight="1">
@@ -56069,7 +56069,7 @@
       <c r="IU1" s="145"/>
       <c r="IV1" s="145"/>
     </row>
-    <row r="2" spans="1:256" ht="15" thickBot="1">
+    <row r="2" spans="1:256" ht="15.75" thickBot="1">
       <c r="A2" s="153" t="str">
         <f>'Сводная таблица'!D2</f>
         <v>Группы 114 05 115 - 114 05 215</v>
@@ -56126,7 +56126,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:256" ht="15" thickBot="1">
+    <row r="4" spans="1:256" ht="15.75" thickBot="1">
       <c r="A4" s="155"/>
       <c r="B4" s="157"/>
       <c r="C4" s="159"/>
@@ -57902,7 +57902,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:11" s="77" customFormat="1" ht="15" thickBot="1">
+    <row r="46" spans="1:11" s="77" customFormat="1" ht="15.75" thickBot="1">
       <c r="A46" s="79">
         <f>'Сводная таблица'!A46:A47</f>
         <v>42</v>

</xml_diff>